<commit_message>
gui updated as well as comments
</commit_message>
<xml_diff>
--- a/temp.xlsx
+++ b/temp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,76 +469,6 @@
           <t>Email</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Lp_2</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Imie_2</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Nazwisko_2</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Data urodzenia_2</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Miasto_2</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Kraj_2</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Email_2</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Lp_3</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>Imie_3</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>Nazwisko_3</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Data urodzenia_3</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>Miasto_3</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>Kraj_3</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>Email_3</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -574,76 +504,6 @@
           <t>Adam.Nowak1@gmail.com</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>1_2</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Adam_2</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Nowak1_2</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>1.01.2000_2</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>Łódź_2</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>Polska_2</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>Adam.Nowak1@gmail.com_2</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>1_3</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>Adam_3</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>Nowak1_3</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>1.01.2000_3</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>Łódź_3</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>Polska_3</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>Adam.Nowak1@gmail.com_3</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -679,76 +539,6 @@
           <t>Michał.Nowak2@gmail.com</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>2_2</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Michał_2</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Nowak2_2</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>1.01.2001_2</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>Kraków_2</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>Polska_2</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>Michał.Nowak2@gmail.com_2</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>2_3</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>Michał_3</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>Nowak2_3</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>1.01.2001_3</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>Kraków_3</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>Polska_3</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>Michał.Nowak2@gmail.com_3</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -784,76 +574,6 @@
           <t>Mateusz.Nowak3@gmail.com</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>3_2</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Mateusz_2</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Nowak3_2</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>1.01.2002_2</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>Warszawa_2</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>Polska_2</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>Mateusz.Nowak3@gmail.com_2</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>3_3</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>Mateusz_3</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>Nowak3_3</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>1.01.2002_3</t>
-        </is>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>Warszawa_3</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>Polska_3</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>Mateusz.Nowak3@gmail.com_3</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -889,76 +609,6 @@
           <t>Bartłomiej.Nowak4@gmail.com</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>4_2</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Bartłomiej_2</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>Nowak4_2</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>1.01.2003_2</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>Gdynia_2</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>Polska_2</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>Bartłomiej.Nowak4@gmail.com_2</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>4_3</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>Bartłomiej_3</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>Nowak4_3</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>1.01.2003_3</t>
-        </is>
-      </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>Gdynia_3</t>
-        </is>
-      </c>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>Polska_3</t>
-        </is>
-      </c>
-      <c r="U5" t="inlineStr">
-        <is>
-          <t>Bartłomiej.Nowak4@gmail.com_3</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -992,76 +642,6 @@
       <c r="G6" t="inlineStr">
         <is>
           <t>Tomasz.Nowak5@gmail.com</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>5_2</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Tomasz_2</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>Nowak5_2</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>1.01.2004_2</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>Sopot_2</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>Polska_2</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>Tomasz.Nowak5@gmail.com_2</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>5_3</t>
-        </is>
-      </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>Tomasz_3</t>
-        </is>
-      </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>Nowak5_3</t>
-        </is>
-      </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>1.01.2004_3</t>
-        </is>
-      </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>Sopot_3</t>
-        </is>
-      </c>
-      <c r="T6" t="inlineStr">
-        <is>
-          <t>Polska_3</t>
-        </is>
-      </c>
-      <c r="U6" t="inlineStr">
-        <is>
-          <t>Tomasz.Nowak5@gmail.com_3</t>
         </is>
       </c>
     </row>

</xml_diff>